<commit_message>
manage multiple stores on each platform
</commit_message>
<xml_diff>
--- a/apps/pczone/test/support/data/built_template_stores_lazada.xlsx
+++ b/apps/pczone/test/support/data/built_template_stores_lazada.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/achilles/Projects/pczone_umbrella/apps/pczone/test/support/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3AEA1D6-B3DB-AC40-BE70-718A64F1584E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05249F5E-4C7B-CF42-96FD-C06426A517D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19800" xr2:uid="{3B25A3A7-DA03-9248-97DF-0D8929A5ED49}"/>
   </bookViews>
@@ -39,13 +39,13 @@
     <t>store_code</t>
   </si>
   <si>
-    <t>lazada</t>
-  </si>
-  <si>
     <t>built_template_code</t>
   </si>
   <si>
     <t>Máy tính mini PC HP EliteDesk 800 G2 65W core i5 6500</t>
+  </si>
+  <si>
+    <t>lazada:thexeonstore</t>
   </si>
 </sst>
 </file>
@@ -411,8 +411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24A7213C-3027-CF43-9AD1-B693EA08A1BB}">
   <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" customHeight="1"/>
@@ -428,7 +428,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -439,7 +439,7 @@
     </row>
     <row r="2" spans="1:4" ht="22" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -448,7 +448,7 @@
         <v>1907169068</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="22" customHeight="1">

</xml_diff>